<commit_message>
feat(transaction):transaction validation for role pegawai
</commit_message>
<xml_diff>
--- a/build/assets/templates/employee_multiple.xlsx
+++ b/build/assets/templates/employee_multiple.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>NIK</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Alamat KTP</t>
+  </si>
+  <si>
+    <t>PTKP</t>
   </si>
 </sst>
 </file>
@@ -384,31 +387,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -422,33 +425,36 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>